<commit_message>
Put useful drone names for the different sheets
</commit_message>
<xml_diff>
--- a/Python/HEL/data/Drones_Propagation.xlsx
+++ b/Python/HEL/data/Drones_Propagation.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\PRESENTATIONS_REPORTS_AND_MISSIONS\SYMPOSIUM_CONFERENCES\20240916_SPIE2024\spie2024\CODE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\GITHUB_REPOSITORIES\Sandbox\Python\HEL\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D614B36-9389-496B-BDCF-05E6C5F95757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BDB4FA-AEAC-4B49-9182-CB8D7D41A624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{66D518BA-4A41-414E-B35F-9020CADD6206}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{66D518BA-4A41-414E-B35F-9020CADD6206}"/>
   </bookViews>
   <sheets>
-    <sheet name="DRONE1" sheetId="3" r:id="rId1"/>
-    <sheet name="DRONE2" sheetId="4" r:id="rId2"/>
-    <sheet name="DRONE3" sheetId="5" r:id="rId3"/>
+    <sheet name="DJI Phantom 4" sheetId="3" r:id="rId1"/>
+    <sheet name="DJI Mavic 3" sheetId="4" r:id="rId2"/>
+    <sheet name="Custom Drone 1" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -789,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD74123E-0597-4BAA-AA7D-F1AE792A159A}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
@@ -899,7 +899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1B7709-702B-4F54-A3B5-835BBDA57EA2}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
Add values to empty sheet for test purpose
</commit_message>
<xml_diff>
--- a/Python/HEL/data/Drones_Propagation.xlsx
+++ b/Python/HEL/data/Drones_Propagation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\GITHUB_REPOSITORIES\Sandbox\Python\HEL\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BDB4FA-AEAC-4B49-9182-CB8D7D41A624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9749A6-6EA0-496E-9C55-68C1B0455932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{66D518BA-4A41-414E-B35F-9020CADD6206}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{66D518BA-4A41-414E-B35F-9020CADD6206}"/>
   </bookViews>
   <sheets>
     <sheet name="DJI Phantom 4" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="53">
   <si>
     <t>x2</t>
   </si>
@@ -555,7 +555,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:M2"/>
+      <selection sqref="A1:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -897,12 +897,151 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1B7709-702B-4F54-A3B5-835BBDA57EA2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>